<commit_message>
SW requirements were updated.
</commit_message>
<xml_diff>
--- a/docu_borimeter/swrs_borimeter.xlsx
+++ b/docu_borimeter/swrs_borimeter.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\users\F10553C\Documents\Git Repo\borimeter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\users\F10553C\Documents\Git Repo\borimeter\docu_borimeter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>SWRS_BRMTR_001</t>
   </si>
@@ -38,10 +38,55 @@
     <t>Requirement Specification</t>
   </si>
   <si>
-    <t xml:space="preserve">After finishing all trials zip the results, in a uniquely named file. </t>
-  </si>
-  <si>
-    <t>Save the file on the local hard drive in a folder named "Results" and promt the user to send it to Bori via mail.</t>
+    <t>SWRS_BRMTR_003</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>User information and test result shall be stored in a text file.</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>SWRS_BRMTR_001_1</t>
+  </si>
+  <si>
+    <t>The result files(s) shall be archived after finishing the test.</t>
+  </si>
+  <si>
+    <t>Archive name must be unique.</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Archive containing test results shall be saved on local hard drive.</t>
+  </si>
+  <si>
+    <t>The user shall be promted to e-mail the test archive to borbalabc@gmail.com</t>
+  </si>
+  <si>
+    <t>SWRS_BRMTR_004</t>
+  </si>
+  <si>
+    <t>SWRS_BRMTR_004_1</t>
+  </si>
+  <si>
+    <t>The name of the text file must be a unique ID.</t>
+  </si>
+  <si>
+    <t>SWRS_BRMTR_005</t>
+  </si>
+  <si>
+    <t>A unique ID shall be calculated for each user, based on their personal information.</t>
   </si>
 </sst>
 </file>
@@ -87,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -96,19 +141,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <sz val="10"/>
-        <color rgb="FF595959"/>
-        <name val="Calibri"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <b val="0"/>
@@ -131,6 +171,50 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF595959"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF595959"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -186,12 +270,80 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF262626"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF262626"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FF595959"/>
+        <name val="Calibri"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -307,13 +459,13 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Oszkar List Style" pivot="0" count="3">
-      <tableStyleElement type="wholeTable" dxfId="11"/>
-      <tableStyleElement type="headerRow" dxfId="10"/>
-      <tableStyleElement type="totalRow" dxfId="9"/>
+      <tableStyleElement type="wholeTable" dxfId="15"/>
+      <tableStyleElement type="headerRow" dxfId="14"/>
+      <tableStyleElement type="totalRow" dxfId="13"/>
     </tableStyle>
     <tableStyle name="SlicerStyleDark6 2" pivot="0" table="0" count="10">
-      <tableStyleElement type="wholeTable" dxfId="8"/>
-      <tableStyleElement type="headerRow" dxfId="7"/>
+      <tableStyleElement type="wholeTable" dxfId="12"/>
+      <tableStyleElement type="headerRow" dxfId="11"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -569,16 +721,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="wishlist" displayName="wishlist" ref="B2:C4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" totalsRowDxfId="4">
-  <autoFilter ref="B2:C4">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Requirement ID" dataDxfId="0" totalsRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="wishlist" displayName="wishlist" ref="B2:E9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" totalsRowDxfId="8">
+  <tableColumns count="4">
+    <tableColumn id="1" name="Requirement ID" dataDxfId="7" totalsRowDxfId="6">
       <calculatedColumnFormula>ROW()-2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Requirement Specification" dataDxfId="1" totalsRowDxfId="2"/>
+    <tableColumn id="7" name="Requirement Specification" dataDxfId="2" totalsRowDxfId="5"/>
+    <tableColumn id="3" name="Type" dataDxfId="0" totalsRowDxfId="3"/>
+    <tableColumn id="2" name="Status" dataDxfId="1" totalsRowDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="Oszkar List Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -850,42 +1000,131 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="B2:C4"/>
+  <dimension ref="B2:E9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="98.140625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="2:3" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="2:3" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
+    <row r="7" spans="2:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>